<commit_message>
updated transcriptions; next tasks
</commit_message>
<xml_diff>
--- a/transcriptions/transcriptions.xlsx
+++ b/transcriptions/transcriptions.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbob/Dropbox/Bob/Projects/PG GP mapping/making new PG odds/PG TOOLKIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjsol\Documents\GitHub\sublexical-toolkit-prep\transcriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B9DE11-BA1A-AD48-9F39-5B2EDCC3F6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCC4884-4FEA-4B14-88D0-9316CF3D950D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="2520" windowWidth="28980" windowHeight="20300" xr2:uid="{E0D8F6B2-9F22-004B-85A9-1BF49A973210}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E0D8F6B2-9F22-004B-85A9-1BF49A973210}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="144">
   <si>
     <t>a</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>numbers like AA0, AA1 can be ignored for all vowels EXCEPT AH (AH1 and AH0 are not the same!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AH2 is the same as this </t>
   </si>
 </sst>
 </file>
@@ -896,19 +899,19 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.1640625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="31.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>86</v>
       </c>
@@ -925,7 +928,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -942,7 +945,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -956,7 +959,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>89</v>
       </c>
@@ -973,7 +976,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -987,7 +990,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1004,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>91</v>
       </c>
@@ -1014,8 +1017,11 @@
       <c r="D7" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+      <c r="E7" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1080,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="23.25" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
@@ -1119,7 +1125,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>40</v>
       </c>
@@ -1175,7 +1181,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>46</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>54</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>121</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
@@ -1273,7 +1279,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>49</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>128</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>19</v>
       </c>
@@ -1374,7 +1380,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>71</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
@@ -1416,7 +1422,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>75</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>78</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>13</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>82</v>
       </c>
@@ -1486,7 +1492,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>83</v>
       </c>

</xml_diff>